<commit_message>
Tous les tests effectués
</commit_message>
<xml_diff>
--- a/ResRandomAvecGroupe/RandomResultats.xlsx
+++ b/ResRandomAvecGroupe/RandomResultats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UQAC\Cours\Système multi-agents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UQAC\Cours\Système multi-agents\Devoir 1\Devoir1Code\ResRandomAvecGroupe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Coefficient</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Coefficient de variation= Ecart type/Moyenne</t>
+  </si>
+  <si>
+    <t>D (Groupe)</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,25 +498,25 @@
         <v>6</v>
       </c>
       <c r="B2" s="3">
-        <v>2.2000000000000002</v>
+        <v>9.6</v>
       </c>
       <c r="C2" s="3">
-        <v>0.8</v>
+        <v>5.4</v>
       </c>
       <c r="D2" s="3">
-        <v>5.6</v>
+        <v>6.4</v>
       </c>
       <c r="E2" s="3">
         <f>AVERAGE(B2:D2)</f>
-        <v>2.8666666666666667</v>
+        <v>7.1333333333333329</v>
       </c>
       <c r="F2" s="3">
         <f>STDEV(B2:D2)</f>
-        <v>2.4684678108764819</v>
+        <v>2.1939310229205811</v>
       </c>
       <c r="G2">
         <f>F2/E2</f>
-        <v>0.86109342239877273</v>
+        <v>0.30756042377391324</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -521,25 +524,25 @@
         <v>7</v>
       </c>
       <c r="B3" s="5">
-        <v>2.2000000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="C3" s="5">
-        <v>5.4</v>
+        <v>7.8</v>
       </c>
       <c r="D3" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3">
         <f>AVERAGE(B3:D3)</f>
-        <v>4.2</v>
+        <v>2.8666666666666667</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F4" si="0">STDEV(B3:D3)</f>
-        <v>1.7435595774162682</v>
+        <f t="shared" ref="F3:F5" si="0">STDEV(B3:D3)</f>
+        <v>4.2910760111344253</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G4" si="1">F3/E3</f>
-        <v>0.41513323271815911</v>
+        <f t="shared" ref="G3:G5" si="1">F3/E3</f>
+        <v>1.4968869806282878</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -547,25 +550,51 @@
         <v>8</v>
       </c>
       <c r="B4" s="3">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="C4" s="3">
-        <v>3.2</v>
+        <v>5.6</v>
       </c>
       <c r="D4" s="3">
-        <v>4.8</v>
+        <v>7.8</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E3:E4" si="2">AVERAGE(B4:D4)</f>
+        <f t="shared" ref="E4:E5" si="2">AVERAGE(B4:D4)</f>
         <v>5</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>1.9078784028338915</v>
+        <v>3.1432467291003414</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>0.38157568056677832</v>
+        <v>0.62864934582006826</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="2"/>
+        <v>3.7333333333333329</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4189197769195194</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.38006779738915702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>